<commit_message>
fix on the file as agreed
</commit_message>
<xml_diff>
--- a/bin/Files/Testdata.xlsx
+++ b/bin/Files/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -180,10 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -732,7 +738,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="44" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>